<commit_message>
More Tests, Consolidated LINQ, Added Index Func
</commit_message>
<xml_diff>
--- a/FastSearch.xlsx
+++ b/FastSearch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\FastSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFE3100-BC3C-41EA-A300-8EFB761BCAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127D51F8-4C42-4E00-9955-0AA3CD2A4363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{E7B18358-42ED-4B76-8751-3D0FF32E4F52}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Search for phoenix 10000 times using Character Tree took 3585100ns,3.5851ms,0.0035851s</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Search for phoenix 10000 times using MapReduce took 8829807300ns,8829.8073ms,8.8298073s</t>
   </si>
   <si>
-    <t>Search for phoenix 10000 times using Better LINQ took 1296197700ns,1296.1977ms,1.2961977s</t>
-  </si>
-  <si>
-    <t>Search for phoenix 10000 times using LINQ took 1671802800ns,1671.8028ms,1.6718028s</t>
-  </si>
-  <si>
     <t>Search for catherine 10000 times using Character Tree took 3725900ns,3.7259ms,0.0037259s</t>
   </si>
   <si>
@@ -60,12 +54,6 @@
     <t>Search for catherine 10000 times using MapReduce took 11759705300ns,11759.7053ms,11.7597053s</t>
   </si>
   <si>
-    <t>Search for catherine 10000 times using Better LINQ took 1155302400ns,1155.3024ms,1.1553024s</t>
-  </si>
-  <si>
-    <t>Search for catherine 10000 times using LINQ took 1752473600ns,1752.4736ms,1.7524736s</t>
-  </si>
-  <si>
     <t>Character Tree indexed 10000 took 192022000ns,192.022ms,0.192022s</t>
   </si>
   <si>
@@ -75,21 +63,12 @@
     <t>Map Reduce indexed 10000 took 4571800ns,4.5718ms,0.0045718s</t>
   </si>
   <si>
-    <t>Better LINQ indexed 10000 took 39337700ns,39.3377ms,0.0393377s</t>
-  </si>
-  <si>
-    <t>LINQ indexed 10000 took 500ns,0.0005ms,5E-07s</t>
-  </si>
-  <si>
     <t>Load 10M passwords took 1214748400ns,1214.7484ms,1.2147484s</t>
   </si>
   <si>
     <t>LINQ</t>
   </si>
   <si>
-    <t>Better LINQ</t>
-  </si>
-  <si>
     <t>MapReduce</t>
   </si>
   <si>
@@ -117,12 +96,6 @@
     <t>Search for PHOENIX 10000 times using MapReduce took 8942302400ns,8942.3024ms,8.9423024s</t>
   </si>
   <si>
-    <t>Search for PHOENIX 10000 times using Better LINQ took 1351685100ns,1351.6851ms,1.3516851s</t>
-  </si>
-  <si>
-    <t>Search for PHOENIX 10000 times using LINQ took 1645617000ns,1645.617ms,1.645617s</t>
-  </si>
-  <si>
     <t>Search Speed (PHOENIX)</t>
   </si>
   <si>
@@ -133,12 +106,6 @@
   </si>
   <si>
     <t>Search for a 10000 times using MapReduce took 3758244400ns,3758.2444ms,3.7582444s</t>
-  </si>
-  <si>
-    <t>Search for a 10000 times using Better LINQ took 2754213400ns,2754.2134ms,2.7542134s</t>
-  </si>
-  <si>
-    <t>Search for a 10000 times using LINQ took 3047964800ns,3047.9648ms,3.0479648s</t>
   </si>
   <si>
     <t>Search Speed (a)</t>
@@ -165,6 +132,21 @@
       </rPr>
       <t xml:space="preserve"> All times in milliseconds</t>
     </r>
+  </si>
+  <si>
+    <t>Search for a 10000 times using LINQ took 2754213400ns,2754.2134ms,2.7542134s</t>
+  </si>
+  <si>
+    <t>Search for PHOENIX 10000 times using LINQ took 1351685100ns,1351.6851ms,1.3516851s</t>
+  </si>
+  <si>
+    <t>Search for phoenix 10000 times using LINQ took 1296197700ns,1296.1977ms,1.2961977s</t>
+  </si>
+  <si>
+    <t>Search for catherine 10000 times using LINQ took 1155302400ns,1155.3024ms,1.1553024s</t>
+  </si>
+  <si>
+    <t>LINQ indexed 10000 took 39337700ns,39.3377ms,0.0393377s</t>
   </si>
 </sst>
 </file>
@@ -542,262 +524,221 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DC8A29-5AB5-4D23-8762-0EDDCC222635}">
-  <dimension ref="B2:I28"/>
+  <dimension ref="B2:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="20.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
+    <col min="3" max="6" width="20.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="D3" s="1">
-        <v>39.337699999999998</v>
+        <v>4.5717999999999996</v>
       </c>
       <c r="E3" s="1">
-        <v>4.5717999999999996</v>
+        <v>410.62419999999997</v>
       </c>
       <c r="F3" s="1">
-        <v>410.62419999999997</v>
-      </c>
-      <c r="G3" s="1">
         <v>192.02199999999999</v>
       </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
         <v>1751.4736</v>
       </c>
       <c r="D4" s="1">
-        <v>1155.3024</v>
+        <v>11759.7053</v>
       </c>
       <c r="E4" s="1">
-        <v>11759.7053</v>
+        <v>5.5231000000000003</v>
       </c>
       <c r="F4" s="1">
-        <v>5.5231000000000003</v>
-      </c>
-      <c r="G4" s="1">
         <v>3.7259000000000002</v>
       </c>
-      <c r="I4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1">
         <v>1671.8027999999999</v>
       </c>
       <c r="D5" s="1">
-        <v>1296.1976999999999</v>
+        <v>8829.8073000000004</v>
       </c>
       <c r="E5" s="1">
-        <v>8829.8073000000004</v>
+        <v>3.5030999999999999</v>
       </c>
       <c r="F5" s="1">
-        <v>3.5030999999999999</v>
-      </c>
-      <c r="G5" s="1">
         <v>3.5851000000000002</v>
       </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1">
         <v>1645.617</v>
       </c>
       <c r="D6" s="1">
-        <v>1351.6850999999999</v>
+        <v>8942.3024000000005</v>
       </c>
       <c r="E6" s="1">
-        <v>8942.3024000000005</v>
+        <v>3.3422000000000001</v>
       </c>
       <c r="F6" s="1">
-        <v>3.3422000000000001</v>
-      </c>
-      <c r="G6" s="1">
         <v>3.8913000000000002</v>
       </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1">
         <v>3047.9648000000002</v>
       </c>
       <c r="D7" s="1">
-        <v>2754.2134000000001</v>
+        <v>3758.2444</v>
       </c>
       <c r="E7" s="1">
-        <v>3758.2444</v>
+        <v>2508.1821</v>
       </c>
       <c r="F7" s="1">
-        <v>2508.1821</v>
-      </c>
-      <c r="G7" s="1">
         <v>0.3337</v>
       </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="16.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="16.399999999999999" x14ac:dyDescent="0.3">
       <c r="C9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I11" t="s">
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I12" t="s">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I16" t="s">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I17" t="s">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I18" t="s">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I19" t="s">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I20" t="s">
+    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I21" t="s">
+    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I22" t="s">
+    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I28" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C4:G7">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="C4:F7">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -808,8 +749,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:G3">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="C3:F3">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -826,6 +767,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010054EBD27ED9BF1E4BB36A95F3F6987A28" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2a41d8cc0a6549a7caf51c3633475033">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="74ab4f5f-b64a-4469-8387-761523e8d0b8" xmlns:ns4="5913ab3c-5f4c-4b7b-81a5-788564ebdc9f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="452f434b42b41686491482dc5e291913" ns3:_="" ns4:_="">
     <xsd:import namespace="74ab4f5f-b64a-4469-8387-761523e8d0b8"/>
@@ -1054,22 +1010,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8475A380-C3F1-452E-8956-4F529FB4D396}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="5913ab3c-5f4c-4b7b-81a5-788564ebdc9f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="74ab4f5f-b64a-4469-8387-761523e8d0b8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75BBFC47-88CA-4307-9B43-1DDE94FBFF05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAAD4AB7-984C-4E69-9FD3-A15EF06D713A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1086,29 +1052,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75BBFC47-88CA-4307-9B43-1DDE94FBFF05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8475A380-C3F1-452E-8956-4F529FB4D396}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5913ab3c-5f4c-4b7b-81a5-788564ebdc9f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="74ab4f5f-b64a-4469-8387-761523e8d0b8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>